<commit_message>
sisdgf com orgao envolvido
</commit_message>
<xml_diff>
--- a/scripts/saidas/sisdgf/processos_cip.xlsx
+++ b/scripts/saidas/sisdgf/processos_cip.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,239 +473,239 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>600443/2019</t>
+          <t>001795/2024</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE JARDIM DE ANGICOS                                                                                                                                                                                                                      </t>
+          <t>PREFEITURA MUNICIPAL DE CEARÁ-MIRIM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PAULO ROBERTO CHAVES ALVES</t>
+          <t>GEORGE MONTENEGRO SOARES</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>09/04/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Análise de despesas e gestão fiscal municipal.</t>
+          <t>Irregularidades em concurso público de Ceará-Mirim.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Encaminhamento à Diretoria de Controle de Pessoal e Previdência para análise dos quesitos, com sugestão de remessa posterior à Diretoria de Controle de Contas de Governo e Gestão Fiscal.</t>
+          <t>Encaminhamento da Coordenadoria de Instrução Processual à Diretoria de Controle de Pessoal e Previdência (DCP) para pronunciamento conclusivo.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>002957/2018</t>
+          <t>002202/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">CAM.MUN.MACAU                                                                                                                                                                                                                                                  </t>
+          <t>CÂMARA MUNICIPAL DE NATAL</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PAULO ROBERTO CHAVES ALVES</t>
+          <t>GEORGE MONTENEGRO SOARES</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>29/01/2025</t>
+          <t>02/04/2025</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>02/04/2025</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Execução de multa por omissão administrativa.</t>
+          <t>Irregularidades em edital de concurso público.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Encaminhamento ao Ministério Público de Contas para manifestação sobre possível falha processual referente à intimação inadequada.</t>
+          <t>Encaminhamento dos autos à Diretoria de Controle de Pessoal e Previdência (DCP) para pronunciamento conclusivo.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>003119/2021</t>
+          <t>000358/2024</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE PUREZA/RN                                                                                                                                                                                                                              </t>
+          <t>PREFEITURA MUNICIPAL DE AFONSO BEZERRA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MARCO ANTÔNIO DE MORAES RÊGO MONTENEGRO</t>
+          <t>ANTONIO ED SOUZA SANTANA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>09/02/2025</t>
+          <t>21/03/2025</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>08/04/2025</t>
+          <t>02/04/2025</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Adequação de despesas com pessoal ao limite.</t>
+          <t>Irregularidades em operações de crédito municipais.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Encaminhamento ao Ministério Público de Contas para manifestação sobre a matéria.</t>
+          <t>Encaminhamento ao Relator para apreciação e decisão, incluindo a aplicação de multa ao responsável e recomendação à Diretoria de Controle de Infraestrutura e Meio Ambiente para acompanhamento das obras financiadas.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>008222/2014</t>
+          <t>005404/2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREF.MUN.SANTA MARIA                                                                                                                                                                                                                                           </t>
+          <t>PREFEITURA MUNICIPAL DE LAGOA DE VELHOS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>RENATO COSTA DIAS</t>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>23/01/2025</t>
+          <t>02/04/2025</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09/04/2025</t>
+          <t>03/04/2025</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Pedido de reconsideração sobre intempestividade de publicação.</t>
+          <t>Análise das contas do Executivo municipal.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Encaminhamento do processo ao Ministério Público junto ao Tribunal de Contas para manifestação.</t>
+          <t>Encaminhamento à Diretoria de Controle de Contas de Governo e Gestão Fiscal para análise da matéria.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>301296/2022</t>
+          <t>002315/2024</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">SOLL – SERVIÇOS, OBRAS E LOCAÇÕES LTDA                                                                                                                                                                                                                         </t>
+          <t>PREFEITURA MUNICIPAL DE PUREZA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PAULO ROBERTO CHAVES ALVES</t>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>29/01/2025</t>
+          <t>23/01/2025</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>30/04/2025</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Representação sobre terceirização ilícita de mão de obra.</t>
+          <t>Omissão de envio de documentos requisitados pelo MPC.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Encaminhamento dos autos ao Ministério Público Especial para manifestação.</t>
+          <t>Encaminhamento do processo ao Relator para análise e decisão sobre a aplicação de multa e aprimoramento do rito processual em processos futuros.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>002206/2023</t>
+          <t>005118/2021</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">SIGILOSO                                                                                                                                                                                                                                                       </t>
+          <t>PREFEITURA MUNICIPAL DE AFONSO BEZERRA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PAULO ROBERTO CHAVES ALVES</t>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>15/04/2025</t>
+          <t>29/01/2025</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>24/04/2025</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Representação sobre contratação por inexigibilidade de licitação.</t>
+          <t>Omissão na prestação de contas de gestão.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Encaminhamento da Diretoria de Instrução Processual à Diretoria de Controle de Infraestrutura e Meio Ambiente.</t>
+          <t>Encaminhamento à consideração do Relator, propondo a rejeição das alegações de defesa, a desaprovação da matéria e a aplicação de multa ao gestor responsável.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>000406/2019</t>
+          <t>600444/2019</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE SÃO FERNANDO                                                                                                                                                                                                                           </t>
+          <t>TRIBUNAL DE CONTAS DO ESTADO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ANA PAULA DE OLIVEIRA GOMES</t>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -715,219 +715,219 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>08/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Irregularidades na gestão fiscal municipal de 2014.</t>
+          <t>Pedido de reconsideração sobre concurso público municipal.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Encaminhamento ao Ministério Público de Contas para manifestação sobre as irregularidades apontadas.</t>
+          <t>Encaminhamento ao Tribunal de Contas do Estado do Rio Grande do Norte com proposta de rejeição do recurso e manutenção integral do acórdão anterior.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>000358/2024</t>
+          <t>200117/2022</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t>CONSÓRCIO PÚBLICO INTERMUNICIPAL DE SANEAMENTO BÁSICO DA REGIÃO DO MATO GRANDE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ANTONIO ED SOUZA SANTANA</t>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>21/03/2025</t>
+          <t>29/01/2025</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>02/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Operação de crédito municipal com irregularidades.</t>
+          <t>Inadimplência no envio de dados pelo consórcio.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Encaminhamento para citação do ex-prefeito de Afonso Bezerra/RN para apresentação de defesa sobre as irregularidades apontadas.</t>
+          <t>Encaminhamento dos autos à Diretoria de Controle de Pessoal e Previdência para análise técnica e continuidade do trâmite processual.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>000289/2023</t>
+          <t>006542/2018</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t>TRIBUNAL DE CONTAS DO ESTADO</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ANA PAULA DE OLIVEIRA GOMES</t>
+          <t>GEORGE MONTENEGRO SOARES</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>29/01/2025</t>
+          <t>09/01/2025</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>24/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Apuração de irregularidades em contratação emergencial.</t>
+          <t>Sugestão de fonte de recurso para SICONFI.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Encaminhamento da Coordenadoria de Instrução Processual à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para análise técnica.</t>
+          <t>Encaminhamento à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para análise e providências.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>004728/2022</t>
+          <t>200152/2021</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">FRANCINALDO MOREIRA DA SILVA                                                                                                                                                                                                                                   </t>
+          <t>CONSÓRCIO PÚBLICO REGIONAL DE SANEAMENTO BÁSICO DO VALE DO ASSU DO RIO GRANDE DO NORTE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ANA PAULA DE OLIVEIRA GOMES</t>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>23/01/2025</t>
+          <t>29/01/2025</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>09/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Regularidade de contratações temporárias e terceirizações ilícitas.</t>
+          <t>Irregularidades no envio de dados ao TCE.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Encaminhamento dos autos ao Ministério Público de Contas para pronunciamento.</t>
+          <t>Encaminhamento à Diretoria de Controle de Pessoal e Previdência para análise e manifestação sobre os fatos.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>303174/2021</t>
+          <t>200032/2022</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE LAGOA D´ANTA                                                                                                                                                                                                                           </t>
+          <t>PREFEITURA MUNICIPAL DE RUY BARBOSA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>PAULO ROBERTO CHAVES ALVES</t>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>29/01/2025</t>
+          <t>09/01/2025</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>30/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Aplicação de multa por falhas na transição.</t>
+          <t>Atraso no envio de dados ao SIAI.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Encaminhamento ao Ministério Público Especial para manifestação nos autos.</t>
+          <t>Encaminhamento para rejeição das alegações de defesa e aplicação de multa ao gestor responsável, com base no posicionamento técnico da Unidade Instrutiva.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>003382/2020</t>
+          <t>200153/2021</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE TOUROS                                                                                                                                                                                                                                 </t>
+          <t>CONSÓRCIO PÚBLICO INTERMUNICIPAL DE SANEAMENTO BÁSICO DA REGIÃO DO MATO GRANDE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>RENATO COSTA DIAS</t>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>03/04/2025</t>
+          <t>29/01/2025</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Arquivamento por prescrição intercorrente.</t>
+          <t>Apuração de irregularidades no envio de dados.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Encaminhamento do processo ao Ministério Público de Contas para manifestação.</t>
+          <t>Encaminhamento da Diretoria de Instrução Processual à Diretoria de Controle de Pessoal e Previdência (DCP).</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>000371/2019</t>
+          <t>200060/2022</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE LUCRÉCIA                                                                                                                                                                                                                               </t>
+          <t>PREFEITURA MUNICIPAL DE MONTE ALEGRE</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RENATO COSTA DIAS</t>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -937,436 +937,436 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>09/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Apuração de irregularidades na gestão fiscal municipal.</t>
+          <t>Atraso no envio de informações ao SIAI.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Encaminhamento do processo ao Ministério Público de Contas para emissão de parecer.</t>
+          <t>Encaminhamento para rejeição das alegações de defesa do Prefeito de Monte Alegre e aplicação de multa, conforme posicionamento técnico da Unidade Instrutiva.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>303175/2021</t>
+          <t>001983/2023</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE LAGOA D´ANTA                                                                                                                                                                                                                           </t>
+          <t>PREFEITURA MUNICIPAL DE CARAÚBAS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>PAULO ROBERTO CHAVES ALVES</t>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>15/04/2025</t>
+          <t>23/01/2025</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>23/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Apuração de inadimplência em contas de água.</t>
+          <t>Inspeção em contratos e gestão de dívidas.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Encaminhamento à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para análise e manifestação.</t>
+          <t>Encaminhamento ao Relator do Tribunal de Contas para avaliação e julgamento, com proposta de rejeição das defesas e aplicação de sanções administrativas.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>011811/2002</t>
+          <t>001543/2025</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREF.MUN.TIMBAÚBA DOS BATISTAS                                                                                                                                                                                                                                 </t>
+          <t>PREFEITURA MUNICIPAL DE FRANCISCO DANTAS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>23/01/2025</t>
+          <t>30/04/2025</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>09/04/2025</t>
+          <t>07/05/2025</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Arquivamento por prescrição intercorrente.</t>
+          <t>Denúncia de irregularidades em licitações municipais.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Encaminhamento ao Ministério Público de Contas para manifestação em sua competência.</t>
+          <t>Encaminhamento da Unidade de Controle Externo à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para realização de instrução preliminar sumária.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>001879/2024</t>
+          <t>002153/2020</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">INSTITUTO DE PREVIDÊNCIA SOCIAL DOS SERVIDORES DO MUNICÍPIO DE NATAL                                                                                                                                                                                           </t>
+          <t>INSTITUTO PREVIDENCIÁRIO DE SÃO PAULO DO POTENGI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>GEORGE MONTENEGRO SOARES</t>
+          <t>RENATO COSTA DIAS</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>27/03/2025</t>
+          <t>03/04/2025</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>23/04/2025</t>
+          <t>07/05/2025</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Auditoria sobre inadimplências previdenciárias em Natal.</t>
+          <t>Apuração de inadimplência no envio ao SIAI-DP.</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Encaminhamento ao Ministério Público de Contas para análise e emissão de parecer.</t>
+          <t>Encaminhamento ao Gabinete do Conselheiro Relator para continuidade do processo.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>002202/2023</t>
+          <t>003046/2018</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">CÂMARA MUNICIPAL DE NATAL                                                                                                                                                                                                                                      </t>
+          <t>PREFEITURA MUNICIPAL DE BARCELONA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>GEORGE MONTENEGRO SOARES</t>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>02/04/2025</t>
+          <t>29/01/2025</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>02/04/2025</t>
+          <t>07/05/2025</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Irregularidades em edital de concurso público.</t>
+          <t>Omissão na prestação de contas da gestão 2016.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Encaminhamento da Coordenadoria de Instrução Processual à Diretoria de Controle de Pessoal e Previdência para pronunciamento conclusivo.</t>
+          <t>Encaminhamento à consideração do Relator para decisão, com proposta de rejeição das defesas, desaprovação das contas e aplicação de multas aos gestores responsáveis.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>005306/2024</t>
+          <t>000406/2019</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t>PREFEITURA MUNICIPAL DE SÃO FERNANDO</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>04/04/2025</t>
+          <t>23/01/2025</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>23/04/2025</t>
+          <t>08/04/2025</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Apuração de irregularidades em edital cultural.</t>
+          <t>Apuração de irregularidades na gestão fiscal municipal.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Encaminhamento ao Tribunal de Contas da União devido à utilização de recursos federais.</t>
+          <t>Encaminhamento ao Relator para aplicação de multas ao gestor por atraso na alimentação do sistema SIAI e má gestão fiscal no exercício de 2014.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>008145/2003</t>
+          <t>003119/2021</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREF.MUN.LAGOA D´ANTA                                                                                                                                                                                                                                          </t>
+          <t>PREFEITURA MUNICIPAL DE PUREZA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+          <t>MARCO ANTÔNIO DE MORAES RÊGO MONTENEGRO</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>23/01/2025</t>
+          <t>09/02/2025</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>09/04/2025</t>
+          <t>08/04/2025</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Arquivamento por prescrição intercorrente.</t>
+          <t>Redução de despesas com pessoal e conformidade fiscal.</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Encaminhamento dos autos ao Ministério Público de Contas para manifestação.</t>
+          <t>Encaminhamento para abertura de novo prazo para o gestor municipal elaborar documentação específica comprovando as medidas implementadas e planejadas, visando atender integralmente às determinações do Tribunal de Contas.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>301005/2025</t>
+          <t>600212/2020</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">ALTBIT INFORMÁTICA COMÉRCIO E SERVIÇOS LTDA                                                                                                                                                                                                                    </t>
+          <t>INSTITUTO DE PREVIDÊNCIA DO MUNICÍPIO DE SÃO MIGUEL</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+          <t>GEORGE MONTENEGRO SOARES</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>04/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>22/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Possíveis irregularidades em pregão de locação.</t>
+          <t>Apuração de responsabilidade perante a SPREV.</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Encaminhamento da Diretoria de Controle de Contas à Secretaria de Estado da Educação para suspensão cautelar de contrato.</t>
+          <t>Encaminhamento à unidade técnica de controle externo competente para análise minuciosa e específica.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>001294/1999</t>
+          <t>019612/2016</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREF.MUN.RIACHUELO                                                                                                                                                                                                                                             </t>
+          <t>TRIBUNAL DE JUSTIÇA</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>GEORGE MONTENEGRO SOARES</t>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>29/01/2025</t>
+          <t>09/04/2025</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>22/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Arquivamento por prescrição decenal reconhecida.</t>
+          <t>Auditoria sobre construção da sede do TJRN.</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Encaminhamento ao Ministério Público de Contas para análise e emissão de parecer.</t>
+          <t>Encaminhamento à unidade técnica de controle externo competente para análise minuciosa e específica.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>300276/2025</t>
+          <t>000147/2025</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t>PROCURADORIA GERAL DE JUSTIÇA</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MARCO ANTÔNIO DE MORAES RÊGO MONTENEGRO</t>
+          <t>SEM RELATOR</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>03/04/2025</t>
+          <t>18/03/2025</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>23/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Suspensão de pregão para aquisição de informática.</t>
+          <t>Reanálise técnica de auditoria em documentação apresentada.</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Encaminhamento da Diretoria de Controle de Contas de Gestão à Secretaria Municipal de Planejamento para manifestação e ratificação de medida cautelar.</t>
+          <t>Encaminhamento da Coordenadoria de Instrução Processual à unidade técnica de controle externo competente.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>001795/2024</t>
+          <t>004098/2019</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">TRIBUNAL DE CONTAS DO ESTADO DO RN                                                                                                                                                                                                                             </t>
+          <t>CONTROLADORIA GERAL DO ESTADO</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>GEORGE MONTENEGRO SOARES</t>
+          <t>RENATO COSTA DIAS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>10/04/2025</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Irregularidades em concurso público de Ceará-Mirim.</t>
+          <t>Análise de Termo de Ajustamento de Gestão.</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Encaminhamento da Coordenadoria de Instrução Processual à Diretoria de Controle de Pessoal e Previdência.</t>
+          <t>Encaminhamento do processo à unidade técnica de controle externo competente para análise minuciosa e específica.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>005404/2024</t>
+          <t>017557/2016</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE LAGOA DE VELHOS                                                                                                                                                                                                                        </t>
+          <t>GABINETE CIVIL DO GOVERNADOR</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+          <t>GEORGE MONTENEGRO SOARES</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>02/04/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>03/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Análise de contas anuais da gestão municipal.</t>
+          <t>Encaminhamento para análise técnica de unidade competente.</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Encaminhamento da Coordenadoria de Instrução Processual à Diretoria de Controle de Contas de Governo e Gestão Fiscal para análise técnica complementar.</t>
+          <t>Encaminhamento à unidade técnica de controle externo competente para análise minuciosa e específica.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>005230/2024</t>
+          <t>002431/2023</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">PREFEITURA MUNICIPAL DE CAMPO GRANDE                                                                                                                                                                                                                           </t>
+          <t>PREFEITURA MUNICIPAL DE GOVERNADOR DIX-SEPT ROSADO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1376,145 +1376,145 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>25/04/2025</t>
+          <t>14/04/2025</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>28/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Análise das contas municipais sem defesa apresentada.</t>
+          <t>Auditoria sobre infraestrutura da educação municipal.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Encaminhamento dos autos ao Ministério Público de Contas para pronunciamento.</t>
+          <t>Encaminhamento à unidade técnica de controle externo competente para análise minuciosa e específica.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>000760/2025</t>
+          <t>007086/2011</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t xml:space="preserve">PREF.MUN.SÃO GONÇALO DO AMARANTE                                                                                                                                                                                                                               </t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+          <t>GEORGE MONTENEGRO SOARES</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>04/04/2025</t>
+          <t>18/03/2025</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>25/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Denúncia sobre irregularidades na SEEC.</t>
+          <t>Análise de despesas do exercício de 2010.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Encaminhamento da Unidade de Controle Externo à Diretoria de Controle de Pessoal e Previdência para instrução preliminar.</t>
+          <t>Encaminhamento à unidade técnica de controle externo competente para análise minuciosa e específica.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>000546/2023</t>
+          <t>025218/2016</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t>CÂMARA MUNICIPAL DE SANTANA DO SERIDÓ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PAULO ROBERTO CHAVES ALVES</t>
+          <t>GEORGE MONTENEGRO SOARES</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>23/04/2025</t>
+          <t>08/05/2025</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Comunicação sobre irregularidade na gestão fiscal.</t>
+          <t>Irregularidades em nomeações durante período vedado.</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Encaminhamento à Relatoria para deliberação e posterior arquivamento do processo.</t>
+          <t>Encaminhamento ao Relator para julgamento de mérito, com aplicação de multa ao ex-prefeito e recomendação à Diretoria de Controle de Despesa com Pessoal para monitoramento futuro das despesas com pessoal.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>300688/2025</t>
+          <t>600443/2019</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t>TRIBUNAL DE CONTAS DO ESTADO</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>08/04/2025</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>09/04/2025</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Apuração de irregularidade em licitação municipal.</t>
+          <t>Análise de concurso e despesas com pessoal.</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Encaminhamento da Diretoria de Instrução Processual à Diretoria de Controle de Contas para análise preliminar e providências.</t>
+          <t>Encaminhamento dos autos à Diretoria de Controle de Pessoal e Previdência para manifestação sobre os quesitos propostos, com sugestão de remessa posterior à Diretoria de Controle de Contas de Governo e Gestão Fiscal.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>301048/2025</t>
+          <t>008145/2003</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t xml:space="preserve">PREF.MUN.LAGOA D´ANTA                                                                                                                                                                                                                                          </t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1524,96 +1524,2049 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>23/01/2025</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>09/04/2025</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Denúncia sobre transparência na gestão municipal.</t>
+          <t>Arquivamento por prescrição intercorrente.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Encaminhamento à Prefeitura Municipal de Senador Eloi de Souza e arquivamento do processo, com acompanhamento previsto em ação do Plano de Fiscalização Anual.</t>
+          <t>Encaminhamento para arquivamento do processo devido à prescrição intercorrente identificada.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>000705/2025</t>
+          <t>004728/2022</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">xxx                                                                                                                                                                                                                                                            </t>
+          <t>PREFEITURA MUNICIPAL DE PEDRO AVELINO</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>RENATO COSTA DIAS</t>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>15/04/2025</t>
+          <t>23/01/2025</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>09/04/2025</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Denúncia sobre transparência nas contas públicas.</t>
+          <t>Irregularidades em contratações temporárias e terceirização ilícita.</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Encaminhamento à Diretoria de Controle de Contas de Gestão para análise preliminar.</t>
+          <t>Encaminhamento à Conselheira Relatora para decisão sobre rejeição das defesas apresentadas, aplicação de multas ao gestor responsável e assinatura de prazo ao Município para sanar as irregularidades constatadas.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>011811/2002</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PREF.MUN.TIMBAÚBA DOS BATISTAS                                                                                                                                                                                                                                 </t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>09/04/2025</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Arquivamento por prescrição intercorrente.</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Encaminhamento para arquivamento do processo devido à prescrição intercorrente, constatada pela paralisação por mais de três anos sem interrupções válidas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>008222/2014</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE SANTA MARIA</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>RENATO COSTA DIAS</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>09/04/2025</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Pedido de reconsideração sobre penalidade por atraso.</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Encaminhamento à consideração superior para conhecimento do recurso e, no mérito, negativa de provimento, com manutenção integral da decisão anterior.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>000371/2019</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE LUCRÉCIA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>RENATO COSTA DIAS</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>09/04/2025</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Aplicação de multa por envio de dados incorretos.</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Encaminhamento para aplicação de multa ao responsável pelo envio incorreto de dados fiscais no Relatório de Gestão Fiscal, com desconsideração das demais imputações não analisadas tecnicamente.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>302014/2021</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE GOIANINHA</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Denúncia sobre transparência e regularidade administrativa.</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Encaminhamento para arquivamento do processo por ausência de materialidade e relevância dos fatos denunciados.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>003284/2022</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NATAL</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Fraude documental em licitação da Prefeitura.</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Encaminhamento do processo ao Ministério Público Estadual para apuração dos fatos e eventual adoção de providências criminais.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>001380/2023</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE OURO BRANCO</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Irregularidade em dispensa de licitação municipal.</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Encaminhamento à consideração do Relator para rejeição das alegações de defesa e aplicação de multa ao prefeito municipal, com desaprovação da matéria conforme análise técnica.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>004658/2019</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE SÃO GONÇALO DO AMARANTE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Arquivamento de dispensa emergencial por regularidade.</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Encaminhamento para arquivamento do processo pela Unidade Técnica de Controle Externo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>004014/2023</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE GUAMARÉ</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Descumprimento da ordem cronológica de pagamentos.</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Encaminhamento ao Ministério Público Estadual para apuração de possível ilícito penal e aplicação de multa ao ex-prefeito.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>004429/2020</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE JOÃO CÂMARA</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>MARCO ANTÔNIO DE MORAES RÊGO MONTENEGRO</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Atraso no envio da prestação de contas.</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos ao Relator para análise e decisão final, com proposta de aplicação de multa e rejeição das alegações de defesa.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>012267/2017</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE MACAÍBA</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Irregularidades em contratos e possíveis danos ao erário.</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Encaminhamento para citação do Prefeito de Macaíba/RN e das empresas envolvidas com vistas à apresentação de defesa sobre possíveis irregularidades contratuais.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>003105/2023</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CÂMARA MUNICIPAL DE SERRA NEGRA DO NORTE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Apuração de omissão na prestação de contas.</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos ao relator para rejeição das alegações de defesa, desaprovação da matéria, aplicação de multa ao gestor e suspensão da certidão de adimplência até a regularização.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>301435/2025</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SECRETARIA MUNICIPAL DE EDUCAÇÃO DE MOSSORÓ</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Descumprimento de ordem cronológica de pagamentos.</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Unidade de Controle Externo à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para instrução preliminar sumária.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>001553/2025</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE MOSSORÓ</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Irregularidades no Portal da Transparência Municipal.</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Unidade de Controle Externo à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para realização da instrução preliminar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>101358/2021</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MARIA JOSE MARTINS                                                                                                                                                                                                                                             </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>RENATO COSTA DIAS</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Denegação de aposentadoria e monitoramento de decisão.</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos à Diretoria de Registro de Atos de Pessoal para providências relacionadas ao monitoramento da decisão.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>005851/2010</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MINISTÉRIO PÚBLICO DO ESTADO DO RIO GRANDE DO NORT                                                                                                                                                                                                             </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Arquivamento por prescrição intercorrente.</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Encaminhamento para arquivamento do processo devido à ocorrência de prescrição intercorrente.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>002249/2013</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM.MUN.GUAMARÉ                                                                                                                                                                                                                                                </t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Análise de recursos sobre irregularidades administrativas.</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos pedidos de reconsideração ao Tribunal de Contas para manter o Acórdão original, exceto em relação à empresa M.V. Pedroza Jucá, onde se reconhece a nulidade da citação e a prescrição da pretensão punitiva.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>001280/2022</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SECRETARIA MUNICIPAL DE SAÚDE DE NATAL</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Gestão inadequada na política de controle de zoonoses.</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Encaminhamento à Diretoria de Avaliação de Políticas Públicas (DPP) para avaliação da política municipal de controle de zoonoses e aplicação de multa ao gestor responsável.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>001503/2025</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE FLORÂNIA</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Irregularidade na contratação de serviços de engenharia.</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Encaminhamento à Diretoria de Controle de Infraestrutura e Meio Ambiente para avaliação de materialidade, risco e relevância dos fatos e indicação de tratamento no Plano de Fiscalização Anual ou posterior análise.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>001505/2025</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE FLORÂNIA</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Irregularidade em contratação de cooperativa de saúde.</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Encaminhamento à Diretoria de Controle de Pessoal e Previdência para pronunciamento quanto à materialidade, risco e relevância dos fatos apontados.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>005267/2018</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE GUAMARÉ</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ANTONIO ED SOUZA SANTANA</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Arquivamento de denúncia sobre pregão presencial.</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Encaminhamento para arquivamento do processo por ausência de indícios de irregularidades no procedimento licitatório.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>001504/2025</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE FLORÂNIA</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Apuração de irregularidade em nomeação de procurador.</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Encaminhamento à Diretoria de Controle de Pessoal e Previdência para avaliação de materialidade, risco e relevância dos fatos apontados.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>001507/2025</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE FLORÂNIA</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Irregularidade na contratação de transporte escolar.</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Diretoria de Instrução Processual e Controle de Decisões à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para pronunciamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>001506/2025</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE FLORÂNIA</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>13/05/2025</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>20/05/2025</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Apuração de irregularidades em contratação municipal.</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Encaminhamento à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para análise de materialidade, risco, relevância e viabilidade de fiscalização.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>000209/2023</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PROCURADORIA GERAL DE JUSTIÇA                                                                                                                                                                                                                                  </t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>GEORGE MONTENEGRO SOARES</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>21/05/2025</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Pagamento antecipado em contratações públicas irregulares.</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos ao Relator para apreciação das conclusões e propostas de aplicação de sanção ao gestor responsável.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>301005/2025</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SECRETARIA DE ESTADO DA EDUCAÇÃO, DA CULTURA, DO ESPORTE E DO LAZER</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>04/04/2025</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>22/04/2025</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Possíveis irregularidades em pregão de locação.</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Unidade de Controle Externo à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para instrução preliminar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>001294/1999</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PREF.MUN.RIACHUELO                                                                                                                                                                                                                                             </t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>GEORGE MONTENEGRO SOARES</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>22/04/2025</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Arquivamento por prescrição de irregularidades formais.</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Encaminhamento para arquivamento do processo, com envio de cópia dos autos ao Ministério Público Estadual para providências cabíveis.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>300276/2025</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SECRETARIA MUNICIPAL DE ADMINISTRAÇÃO DE NATAL</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>MARCO ANTÔNIO DE MORAES RÊGO MONTENEGRO</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>23/04/2025</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Suspensão de pregão eletrônico por denúncia.</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública (DCD) para pronunciamento conclusivo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>000546/2023</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE JARDIM DE PIRANHAS</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>23/04/2025</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Comunicação de irregularidade sobre gestão fiscal.</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos à Diretoria de Controle de Contas de Governo e Gestão Fiscal para pronunciamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>303175/2021</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE LAGOA D´ANTA</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>15/04/2025</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>23/04/2025</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Responsabilização administrativa por inadimplência em gestão.</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos à Diretoria de Controle de Contas de Gestão para apuração do dano ao erário e análise da conduta da ex-prefeita, com citação da mesma para apresentação de defesa.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>005306/2024</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE MACAU</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>04/04/2025</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>23/04/2025</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Denúncia sobre irregularidades em edital cultural.</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Unidade de Controle Externo à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para instrução preliminar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>001879/2024</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>INSTITUTO DE PREVIDÊNCIA SOCIAL DOS SERVIDORES DO MUNICÍPIO DE NATAL</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>GEORGE MONTENEGRO SOARES</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>27/03/2025</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>23/04/2025</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Auditoria sobre inadimplência previdenciária em Natal.</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Encaminhamento à apreciação do Relator para decisão sobre aplicação de sanções aos responsáveis e fixação de prazo para regularização das pendências previdenciárias.</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>003103/2023</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE RAFAEL FERNANDES</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>27/02/2025</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>23/05/2025</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Omissão na prestação de contas anuais.</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Encaminhamento ao Relator com proposta de rejeição das alegações de defesa, desaprovação da matéria, aplicação de multa ao gestor e suspensão da Certidão de Adimplência enquanto persistir a irregularidade.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>001317/2017</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>TRIBUNAL DE CONTAS DO ESTADO</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>ANTONIO ED SOUZA SANTANA</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>23/05/2025</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>23/05/2025</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Monitoramento de auditoria do sistema prisional.</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Encaminhamento do processo à Diretoria de Avaliação de Políticas Públicas para análise do Plano de Ação e inclusão em ação fiscalizatória no Plano de Fiscalização Anual.</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>002206/2023</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SECRETARIA DE ESTADO DA SAÚDE PUBLICA</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>15/04/2025</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>24/04/2025</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Apuração de irregularidades em contratação sem licitação.</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Coordenadoria de Instrução Processual à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para pronunciamento conclusivo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>000289/2023</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE OURO BRANCO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>ANA PAULA DE OLIVEIRA GOMES</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>24/04/2025</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Apuração de irregularidades em transporte escolar.</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Encaminhamento à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para análise e pronunciamento técnico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>000760/2025</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SECRETARIA DE ESTADO DA EDUCAÇÃO, DA CULTURA, DO ESPORTE E DO LAZER</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>04/04/2025</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>25/04/2025</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Denúncia sobre transparência em contratações temporárias.</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Encaminhamento à Diretoria de Controle de Pessoal e Previdência para realização de instrução preliminar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
           <t>001039/2025</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">COMPANHIA POTIGUAR DE GÁS - POTIGÁS                                                                                                                                                                                                                            </t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>COMPANHIA POTIGUAR DE GÁS</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
         <is>
           <t>SEM RELATOR</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>23/04/2025</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>25/04/2025</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Inclusão do GNV em relatório de licitação.</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Encaminhamento de ofício da Companhia Potiguar de Gás à Diretoria de Expediente para apensamento e aguardo de resposta à notificação.</t>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Inclusão do GNV em relatório de transporte.</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Encaminhamento do documento ao gabinete do Conselheiro Relator para apensamento aos autos do processo relacionado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>006450/2017</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE PORTO DO MANGUE</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>10/01/2025</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>27/05/2025</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Fixação irregular de subsídios de agentes políticos.</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos ao Relator para julgamento de irregularidade da matéria e aplicação das penalidades propostas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>001981/2023</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE UMARIZAL</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>27/05/2025</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>27/05/2025</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Irregularidades em contratos e gestão de dívidas.</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Encaminhamento ao Relator para apreciação e decisão quanto à desaprovação da matéria, imputação de débito solidário aos gestores e aplicação das penalidades propostas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>005230/2024</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE CAMPO GRANDE</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>25/04/2025</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>28/04/2025</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Análise de contas do prefeito sem defesa.</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Encaminhamento ao gabinete do Conselheiro Relator para decretação de revelia do responsável e posterior envio ao Ministério Público de Contas para pronunciamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>011897/2011</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM.MUN.SÃO GONÇALO DO AMARANTE                                                                                                                                                                                                                                </t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>GEORGE MONTENEGRO SOARES</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>28/05/2025</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Arquivamento por prescrição decenal.</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos ao Conselheiro Relator para reconhecimento da prescrição e arquivamento do processo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>003382/2020</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE TOUROS</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>RENATO COSTA DIAS</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Arquivamento por prescrição intercorrente.</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Encaminhamento para arquivamento do processo devido à ocorrência de prescrição intercorrente.</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>301048/2025</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE SEN.ELOI DE SOUZA</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Denúncia sobre descumprimento do dever de transparência.</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Unidade de Controle Externo à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para instrução preliminar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>000705/2025</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE SERRINHA</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>RENATO COSTA DIAS</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>15/04/2025</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Denúncia sobre transparência das contas públicas.</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Diretoria de Instrução Processual à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública (DCD) para instrução preliminar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>002957/2018</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>CÂMARA MUNICIPAL DE MACAU</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Execução de multa por omissão na gestão.</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Encaminhamento à adoção de medidas para fixação do limite máximo da multa e execução forçada do débito acumulado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>300688/2025</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE SÃO MIGUEL DE GOSTOSO</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>ANTONIO GILBERTO DE OLIVEIRA JALES</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>08/04/2025</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Denúncia sobre irregularidade em licitação municipal.</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Encaminhamento da Unidade de Controle Externo à Diretoria de Controle de Contas de Gestão e Execução da Despesa Pública para a instrução preliminar sumária.</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>005179/2019</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE BARAÚNA</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>23/01/2025</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>29/05/2025</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Pedido de reconsideração sobre omissão na prestação de contas.</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Encaminhamento do recurso de Pedido de Reconsideração para análise superior, com proposta de manutenção integral da decisão recorrida.</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>005114/2021</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>CÂMARA MUNICIPAL DE LAGOA D´ANTA</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>29/05/2025</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Omissão na prestação de contas de gestão.</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Encaminhamento ao Relator para rejeição das alegações de defesa, desaprovação da matéria, aplicação de multa ao gestor e suspensão da Certidão de Adimplência.</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>002322/2024</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NATAL</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>GEORGE MONTENEGRO SOARES</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>27/05/2025</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>29/05/2025</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Acompanhamento de licitação de transporte coletivo.</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos à Diretoria de Controle de Infraestrutura e Meio Ambiente para manifestação, conforme determinação do Relator.</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>017609/2016</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>CÂMARA MUNICIPAL DE PEDRO AVELINO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>GEORGE MONTENEGRO SOARES</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>09/02/2025</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>29/05/2025</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Irregularidades em remunerações na Câmara Municipal.</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos ao Ministério Público de Contas para pronunciamento conclusivo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>301296/2022</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE MONTE ALEGRE</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>30/04/2025</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Contratação irregular de cooperativa para serviços educacionais.</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Encaminhamento ao Relator para análise das defesas, aplicação de multa ao ex-gestor e fixação de prazo ao Município para regularização das irregularidades constatadas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>303174/2021</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE LAGOA D´ANTA</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>PAULO ROBERTO CHAVES ALVES</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>29/01/2025</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>30/04/2025</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Descumprimento de normas na transição administrativa municipal.</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Encaminhamento dos autos ao Relator para decisão, com proposta de aplicação de multa à ex-prefeita e suspensão da certidão de adimplência.</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>005354/2024</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE JAPI</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>ANTONIO ED SOUZA SANTANA</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Apensamento de documento sobre contas executivas municipais.</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Apensamento de documento ao processo para análise das contas do Chefe do Poder Executivo da Prefeitura Municipal de Japi.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>000739/2023</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>GOVERNO DO ESTADO DO RN</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>FRANCISCO POTIGUAR CAVALCANTI JÚNIOR</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>03/02/2025</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Acompanhamento do uso do SIGEF como SIAFIC.</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Apensamento de documento ao processo em acompanhamento no Tribunal de Contas do Estado do Rio Grande do Norte.</t>
         </is>
       </c>
     </row>

</xml_diff>